<commit_message>
se agrega dato de encla 2019
</commit_message>
<xml_diff>
--- a/Output/cuadro1.Empresas_con_sindicato.xlsx
+++ b/Output/cuadro1.Empresas_con_sindicato.xlsx
@@ -1,47 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://inechile-my.sharepoint.com/personal/nicolas_ratto_ine_cl/Documents/GitHub/OBSERVATORIO SINDICAL/Encla histórica/Output/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="11_CF7BFDCE8F79A8D366075C52F3881A77B31D994F" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E7B58FBF-5EDA-4D3A-A392-11281AC04732}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>ano</t>
-  </si>
-  <si>
-    <t>sin_sindicato</t>
-  </si>
-  <si>
-    <t>con_sindicato</t>
-  </si>
-  <si>
-    <t>porcentaje_sindicato</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -51,13 +25,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -82,39 +49,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Millares [0]" xfId="1" builtinId="6"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentaje" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -156,7 +109,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -188,27 +141,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -240,24 +175,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -433,142 +350,159 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="4" max="4" width="10.7265625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ano</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>sin_sindicato</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>con_sindicato</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>porcentaje_sindicato</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2">
         <v>1998</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2">
         <v>985</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2">
         <v>256</v>
       </c>
-      <c r="D2" s="2">
-        <v>0.20628525382755841</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D2">
+        <v>0.2062852538275584</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3">
         <v>1999</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3">
         <v>1025</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3">
         <v>220</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3">
         <v>0.1764234161988773</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4">
       <c r="A4">
         <v>2002</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4">
         <v>974</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4">
         <v>179</v>
       </c>
-      <c r="D4" s="2">
-        <v>0.15524718126626191</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D4">
+        <v>0.1552471812662619</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5">
         <v>2004</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5">
         <v>1052</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5">
         <v>131</v>
       </c>
-      <c r="D5" s="2">
-        <v>0.11073541842772611</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D5">
+        <v>0.1107354184277261</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6">
         <v>2006</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6">
         <v>1179</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6">
         <v>102</v>
       </c>
-      <c r="D6" s="2">
-        <v>7.9625292740046844E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D6">
+        <v>0.07962529274004684</v>
+      </c>
+    </row>
+    <row r="7">
       <c r="A7">
         <v>2008</v>
       </c>
-      <c r="B7" s="3">
-        <v>82860.181539044002</v>
-      </c>
-      <c r="C7" s="3">
-        <v>4714.7084394940002</v>
-      </c>
-      <c r="D7" s="2">
-        <v>5.3836304454957747E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B7">
+        <v>82860.181539044</v>
+      </c>
+      <c r="C7">
+        <v>4714.708439494</v>
+      </c>
+      <c r="D7">
+        <v>0.05383630445495775</v>
+      </c>
+    </row>
+    <row r="8">
       <c r="A8">
         <v>2011</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8">
         <v>70208.39941759748</v>
       </c>
-      <c r="C8" s="3">
-        <v>6128.9940485078114</v>
-      </c>
-      <c r="D8" s="2">
-        <v>8.028822796037903E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C8">
+        <v>6128.994048507811</v>
+      </c>
+      <c r="D8">
+        <v>0.08028822796037903</v>
+      </c>
+    </row>
+    <row r="9">
       <c r="A9">
         <v>2014</v>
       </c>
-      <c r="B9" s="3">
-        <v>74560.964072917501</v>
-      </c>
-      <c r="C9" s="3">
-        <v>5110.6573967782178</v>
-      </c>
-      <c r="D9" s="2">
-        <v>6.4146521716294327E-2</v>
+      <c r="B9">
+        <v>74560.9640729175</v>
+      </c>
+      <c r="C9">
+        <v>5110.657396778218</v>
+      </c>
+      <c r="D9">
+        <v>0.06414652171629433</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>2019</v>
+      </c>
+      <c r="B10">
+        <v>4987.260261524349</v>
+      </c>
+      <c r="C10">
+        <v>74449.40836741091</v>
+      </c>
+      <c r="D10">
+        <v>0.06278284761437881</v>
       </c>
     </row>
   </sheetData>

</xml_diff>